<commit_message>
Update profile and rebuild IG
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-PRAT-Encounter.xlsx
+++ b/output/StructureDefinition-PRAT-Encounter.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$89</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2846" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3090" uniqueCount="507">
   <si>
     <t>Path</t>
   </si>
@@ -729,7 +729,7 @@
     <t>The entity structuring the timepoint</t>
   </si>
   <si>
-    <t>The nature and cadence of a timepoint can be structured by entities external or specific to a given provider, like a Payer that mandates certain assessments be completed</t>
+    <t>The nature and cadence of a timepoint can be structured by entities external or specific to a given provider, like a Payer that mandates certain assessments be completed.</t>
   </si>
   <si>
     <t>Since there are many ways to further classify encounters, this element is 0..*.</t>
@@ -857,7 +857,7 @@
 </t>
   </si>
   <si>
-    <t>Clinical Impression can reflect any and all clinical related data tied to the assessment/instrument driving the timepoint, or within the timepoint itself</t>
+    <t>The ServiceRequest that initiated this encounter</t>
   </si>
   <si>
     <t>The request this encounter satisfies (e.g. incoming referral or procedure request).</t>
@@ -869,13 +869,109 @@
     <t>.reason.ClinicalDocument</t>
   </si>
   <si>
+    <t>Encounter.basedOn.id</t>
+  </si>
+  <si>
+    <t>Encounter.basedOn.extension</t>
+  </si>
+  <si>
+    <t>impression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/pacio-rat/StructureDefinition/clinicalImpression}
+</t>
+  </si>
+  <si>
+    <t>Clinical Impression can reflect any and all clinical related data tied to the assessment/instrument driving the timepoint, or within the timepoint itself.</t>
+  </si>
+  <si>
+    <t>Clinical impression resource reference</t>
+  </si>
+  <si>
+    <t>Encounter.basedOn.reference</t>
+  </si>
+  <si>
+    <t>Literal reference, Relative, internal or absolute URL</t>
+  </si>
+  <si>
+    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
+  </si>
+  <si>
+    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
+  </si>
+  <si>
+    <t>Reference.reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref-1
+</t>
+  </si>
+  <si>
+    <t>Encounter.basedOn.type</t>
+  </si>
+  <si>
+    <t>Type the reference refers to (e.g. "Patient")</t>
+  </si>
+  <si>
+    <t>The expected type of the target of the reference. If both Reference.type and Reference.reference are populated and Reference.reference is a FHIR URL, both SHALL be consistent.
+The type is the Canonical URL of Resource Definition that is the type this reference refers to. References are URLs that are relative to http://hl7.org/fhir/StructureDefinition/ e.g. "Patient" is a reference to http://hl7.org/fhir/StructureDefinition/Patient. Absolute URLs are only allowed for logical models (and can only be used in references in logical models, not resources).</t>
+  </si>
+  <si>
+    <t>This element is used to indicate the type of  the target of the reference. This may be used which ever of the other elements are populated (or not). In some cases, the type of the target may be determined by inspection of the reference (e.g. a RESTful URL) or by resolving the target of the reference; if both the type and a reference is provided, the reference SHALL resolve to a resource of the same type as that specified.</t>
+  </si>
+  <si>
+    <t>Aa resource (or, for logical models, the URI of the logical model).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/resource-types</t>
+  </si>
+  <si>
+    <t>Reference.type</t>
+  </si>
+  <si>
+    <t>Encounter.basedOn.identifier</t>
+  </si>
+  <si>
+    <t>Logical reference, when literal reference is not known</t>
+  </si>
+  <si>
+    <t>An identifier for the target resource. This is used when there is no way to reference the other resource directly, either because the entity it represents is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
+  </si>
+  <si>
+    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
+When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
+Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.
+Reference is intended to point to a structure that can potentially be expressed as a FHIR resource, though there is no need for it to exist as an actual FHIR resource instance - except in as much as an application wishes to actual find the target of the reference. The content referred to be the identifier must meet the logical constraints implied by any limitations on what resource types are permitted for the reference.  For example, it would not be legitimate to send the identifier for a drug prescription if the type were Reference(Observation|DiagnosticReport).  One of the use-cases for Reference.identifier is the situation where no FHIR representation exists (where the type is Reference (Any).</t>
+  </si>
+  <si>
+    <t>Reference.identifier</t>
+  </si>
+  <si>
+    <t>.identifier</t>
+  </si>
+  <si>
+    <t>Encounter.basedOn.display</t>
+  </si>
+  <si>
+    <t>Text alternative for the resource</t>
+  </si>
+  <si>
+    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
+  </si>
+  <si>
+    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
+  </si>
+  <si>
+    <t>Reference.display</t>
+  </si>
+  <si>
     <t>Encounter.participant</t>
   </si>
   <si>
     <t>Clinicians or Care Teams active in a timepoint</t>
   </si>
   <si>
-    <t>Any clinicians or other team members who had an interaction with a patient during a given time point period</t>
+    <t>Any clinicians or other team members who had an interaction with a patient during a given time point period.</t>
   </si>
   <si>
     <t>Event.performer</t>
@@ -967,10 +1063,7 @@
 </t>
   </si>
   <si>
-    <t>The appointment that scheduled this encounter</t>
-  </si>
-  <si>
-    <t>The appointment that scheduled this encounter.</t>
+    <t>Scheduled appointment or appointments that start the timepoint.</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode=FLFS].target[classCode=ENC, moodCode=APT]</t>
@@ -985,7 +1078,7 @@
     <t>The start and end date/time of the timepoint</t>
   </si>
   <si>
-    <t>The start and end time of the encounter.</t>
+    <t>The start and end date/time of the timepoint.</t>
   </si>
   <si>
     <t>If not (yet) known, the end of the Period may be omitted.</t>
@@ -1010,10 +1103,7 @@
 </t>
   </si>
   <si>
-    <t>Quantity of time the encounter lasted (less time absent)</t>
-  </si>
-  <si>
-    <t>Quantity of time the encounter lasted. This excludes the time during leaves of absence.</t>
+    <t>Days in a given timepoint period.</t>
   </si>
   <si>
     <t>May differ from the time the Encounter.period lasted because of leave of absence.</t>
@@ -1032,10 +1122,10 @@
 Admission diagnosis</t>
   </si>
   <si>
-    <t>the ICD or Snomed Code that is the subject of the given timepoint</t>
-  </si>
-  <si>
-    <t>ICD 10 code is preferred in this field, and should reflect the focus of the timepoint. If the focus of the timepoint is a Home Health OASIS, then the Primary Diagnosis would be the reason code. If the focus is therapy related, then the reason should reflect the ICD Code(s) being treated by the therapist</t>
+    <t>The ICD or Snomed Code that is the subject of the given timepoint</t>
+  </si>
+  <si>
+    <t>ICD 10 code is preferred in this field, and should reflect the focus of the timepoint. If the focus of the timepoint is a Home Health OASIS, then the Primary Diagnosis would be the reason code. If the focus is therapy related, then the reason should reflect the ICD Code(s) being treated by the therapist.</t>
   </si>
   <si>
     <t>For systems that need to know which was the primary diagnosis, these will be marked with the standard extension primaryDiagnosis (which is a sequence value rather than a flag, 1 = primary diagnosis).</t>
@@ -1075,10 +1165,7 @@
     <t>Encounter.diagnosis</t>
   </si>
   <si>
-    <t>The list of diagnosis relevant to this encounter</t>
-  </si>
-  <si>
-    <t>The list of diagnosis relevant to this encounter.</t>
+    <t>Holding all DX codes for given patient during a given timepoint.</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode=RSON]</t>
@@ -1394,7 +1481,7 @@
     <t>Encounter.location.location</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Location)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-location)
 </t>
   </si>
   <si>
@@ -1465,6 +1552,10 @@
     <t>Encounter.serviceProvider</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization)
+</t>
+  </si>
+  <si>
     <t>The organization (facility) responsible for this encounter</t>
   </si>
   <si>
@@ -1480,7 +1571,7 @@
     <t>Encounter.partOf</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Encounter)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter)
 </t>
   </si>
   <si>
@@ -1647,7 +1738,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM82"/>
+  <dimension ref="A1:AM89"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1656,45 +1747,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="44.59765625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="61.51171875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="45.671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="63.671875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="133.296875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="138.08203125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="95.39453125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="56.90625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="44.59765625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="98.375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="56.25" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="45.671875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="26.6875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="99.8984375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="33.046875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="187.4921875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="29.69921875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="102.6171875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="191.12890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2823,7 +2914,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>42</v>
@@ -3923,7 +4014,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>189</v>
       </c>
@@ -3939,7 +4030,7 @@
         <v>42</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>43</v>
@@ -5465,7 +5556,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
         <v>236</v>
       </c>
@@ -5481,7 +5572,7 @@
         <v>50</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>43</v>
@@ -5794,7 +5885,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
         <v>260</v>
       </c>
@@ -5810,7 +5901,7 @@
         <v>42</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>43</v>
@@ -5903,7 +5994,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
         <v>267</v>
       </c>
@@ -5913,13 +6004,13 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F39" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>43</v>
@@ -6012,7 +6103,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
         <v>274</v>
       </c>
@@ -6025,25 +6116,25 @@
         <v>41</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>190</v>
+        <v>52</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>275</v>
+        <v>116</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>276</v>
+        <v>117</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6094,47 +6185,47 @@
         <v>43</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>274</v>
+        <v>118</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>277</v>
+        <v>43</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>278</v>
+        <v>119</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>279</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>43</v>
@@ -6146,15 +6237,17 @@
         <v>43</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="M41" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>99</v>
+      </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>43</v>
@@ -6191,31 +6284,31 @@
         <v>43</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="AB41" t="s" s="2">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="AC41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD41" t="s" s="2">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>43</v>
@@ -6230,13 +6323,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" hidden="true">
+    <row r="42">
       <c r="A42" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="B42" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>276</v>
+      </c>
       <c r="C42" t="s" s="2">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6246,7 +6341,7 @@
         <v>42</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>43</v>
@@ -6255,17 +6350,15 @@
         <v>43</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>96</v>
+        <v>277</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>97</v>
+        <v>278</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>99</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>43</v>
@@ -6332,7 +6425,7 @@
         <v>43</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>43</v>
@@ -6343,43 +6436,41 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>197</v>
+        <v>43</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I43" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>198</v>
+        <v>281</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>199</v>
+        <v>282</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>43</v>
       </c>
@@ -6427,19 +6518,19 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>200</v>
+        <v>284</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>43</v>
+        <v>285</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>43</v>
@@ -6454,9 +6545,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6467,10 +6558,10 @@
         <v>41</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>43</v>
@@ -6479,16 +6570,16 @@
         <v>51</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>137</v>
+        <v>64</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6517,10 +6608,10 @@
         <v>142</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>43</v>
@@ -6538,13 +6629,13 @@
         <v>43</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>43</v>
@@ -6553,21 +6644,21 @@
         <v>62</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>288</v>
+        <v>43</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>289</v>
+        <v>93</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>290</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6581,24 +6672,26 @@
         <v>50</v>
       </c>
       <c r="G45" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I45" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H45" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I45" t="s" s="2">
-        <v>43</v>
-      </c>
       <c r="J45" t="s" s="2">
-        <v>165</v>
+        <v>108</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="M45" s="2"/>
+        <v>295</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>296</v>
+      </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>43</v>
@@ -6647,7 +6740,7 @@
         <v>43</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6665,18 +6758,18 @@
         <v>43</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>295</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6690,7 +6783,7 @@
         <v>50</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>43</v>
@@ -6699,15 +6792,17 @@
         <v>51</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>297</v>
+        <v>52</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="M46" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>302</v>
+      </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>43</v>
@@ -6756,7 +6851,7 @@
         <v>43</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6771,19 +6866,19 @@
         <v>62</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>300</v>
+        <v>43</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>301</v>
+        <v>93</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>302</v>
+        <v>43</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>303</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="47" hidden="true">
+    <row r="47">
       <c r="A47" t="s" s="2">
         <v>304</v>
       </c>
@@ -6793,13 +6888,13 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>43</v>
@@ -6808,13 +6903,13 @@
         <v>51</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="K47" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K47" t="s" s="2">
+      <c r="L47" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6880,7 +6975,7 @@
         <v>62</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>272</v>
+        <v>307</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>308</v>
@@ -6892,7 +6987,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
         <v>310</v>
       </c>
@@ -6908,7 +7003,7 @@
         <v>50</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>43</v>
@@ -6917,17 +7012,15 @@
         <v>43</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>311</v>
+        <v>116</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>313</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>43</v>
@@ -6976,7 +7069,7 @@
         <v>43</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>310</v>
+        <v>118</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6988,35 +7081,35 @@
         <v>43</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>314</v>
+        <v>43</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>315</v>
+        <v>119</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>316</v>
+        <v>43</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>317</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>43</v>
@@ -7028,16 +7121,16 @@
         <v>43</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>319</v>
+        <v>96</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>320</v>
+        <v>97</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>321</v>
+        <v>121</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>322</v>
+        <v>99</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -7087,40 +7180,40 @@
         <v>43</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>318</v>
+        <v>125</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>314</v>
+        <v>43</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>323</v>
+        <v>119</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>324</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>326</v>
+        <v>197</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7130,27 +7223,29 @@
         <v>42</v>
       </c>
       <c r="G50" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H50" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="H50" t="s" s="2">
-        <v>43</v>
       </c>
       <c r="I50" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>327</v>
+        <v>198</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>328</v>
+        <v>199</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="N50" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="O50" t="s" s="2">
         <v>43</v>
       </c>
@@ -7174,13 +7269,13 @@
         <v>43</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>330</v>
+        <v>43</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>331</v>
+        <v>43</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>43</v>
@@ -7198,7 +7293,7 @@
         <v>43</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>325</v>
+        <v>200</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7210,28 +7305,28 @@
         <v>43</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>332</v>
+        <v>43</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>333</v>
+        <v>93</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>334</v>
+        <v>43</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>335</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>326</v>
+        <v>43</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -7250,16 +7345,16 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>337</v>
+        <v>137</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7285,13 +7380,13 @@
         <v>43</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>43</v>
+        <v>315</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>43</v>
+        <v>317</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>43</v>
@@ -7309,7 +7404,7 @@
         <v>43</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7324,21 +7419,21 @@
         <v>62</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>334</v>
+        <v>43</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
-    <row r="52" hidden="true">
+    <row r="52">
       <c r="A52" t="s" s="2">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7349,25 +7444,25 @@
         <v>41</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7418,13 +7513,13 @@
         <v>43</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>43</v>
@@ -7436,18 +7531,18 @@
         <v>43</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>43</v>
+        <v>325</v>
       </c>
     </row>
-    <row r="53" hidden="true">
+    <row r="53">
       <c r="A53" t="s" s="2">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7461,22 +7556,22 @@
         <v>50</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I53" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>52</v>
+        <v>327</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>116</v>
+        <v>328</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>117</v>
+        <v>329</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7527,7 +7622,7 @@
         <v>43</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>118</v>
+        <v>326</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7539,28 +7634,28 @@
         <v>43</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>43</v>
+        <v>330</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>119</v>
+        <v>331</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>43</v>
+        <v>332</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>43</v>
+        <v>333</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
@@ -7576,20 +7671,18 @@
         <v>43</v>
       </c>
       <c r="I54" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>96</v>
+        <v>335</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>97</v>
+        <v>336</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>99</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
         <v>43</v>
@@ -7638,7 +7731,7 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>125</v>
+        <v>334</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7650,60 +7743,58 @@
         <v>43</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>43</v>
+        <v>272</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>119</v>
+        <v>337</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>43</v>
+        <v>338</v>
       </c>
     </row>
-    <row r="55" hidden="true">
+    <row r="55">
       <c r="A55" t="s" s="2">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>197</v>
+        <v>43</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>198</v>
+        <v>340</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>199</v>
+        <v>341</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
         <v>43</v>
       </c>
@@ -7751,31 +7842,31 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>200</v>
+        <v>339</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG55" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH55" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>43</v>
+        <v>343</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>93</v>
+        <v>344</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>43</v>
+        <v>345</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>43</v>
+        <v>346</v>
       </c>
     </row>
     <row r="56" hidden="true">
@@ -7784,11 +7875,11 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>348</v>
+        <v>43</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F56" t="s" s="2">
         <v>50</v>
@@ -7800,19 +7891,19 @@
         <v>43</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -7865,7 +7956,7 @@
         <v>347</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>50</v>
@@ -7877,52 +7968,54 @@
         <v>62</v>
       </c>
       <c r="AJ56" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM56" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="AK56" t="s" s="2">
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="57" hidden="true">
-      <c r="A57" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>43</v>
+        <v>354</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J57" t="s" s="2">
         <v>137</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
         <v>43</v>
@@ -7971,13 +8064,13 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH57" t="s" s="2">
         <v>43</v>
@@ -7986,52 +8079,54 @@
         <v>62</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>43</v>
+        <v>360</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>119</v>
+        <v>361</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>43</v>
+        <v>362</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>43</v>
+        <v>363</v>
       </c>
     </row>
-    <row r="58" hidden="true">
+    <row r="58">
       <c r="A58" t="s" s="2">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>43</v>
+        <v>354</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="M58" s="2"/>
+        <v>367</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>357</v>
+      </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
         <v>43</v>
@@ -8080,13 +8175,13 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>43</v>
@@ -8095,21 +8190,21 @@
         <v>62</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>43</v>
+        <v>360</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>43</v>
+        <v>362</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>43</v>
+        <v>363</v>
       </c>
     </row>
-    <row r="59" hidden="true">
+    <row r="59">
       <c r="A59" t="s" s="2">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8117,32 +8212,30 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F59" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>366</v>
+        <v>190</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="M59" t="s" s="2">
         <v>369</v>
       </c>
+      <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>43</v>
@@ -8191,7 +8284,7 @@
         <v>43</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8218,7 +8311,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
         <v>371</v>
       </c>
@@ -8234,7 +8327,7 @@
         <v>50</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>43</v>
@@ -8243,17 +8336,15 @@
         <v>43</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>190</v>
+        <v>52</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>372</v>
+        <v>116</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>374</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>43</v>
@@ -8302,7 +8393,7 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>371</v>
+        <v>118</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8314,13 +8405,13 @@
         <v>43</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>375</v>
+        <v>119</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>43</v>
@@ -8331,18 +8422,18 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>43</v>
@@ -8354,15 +8445,17 @@
         <v>43</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="M61" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>99</v>
+      </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>43</v>
@@ -8411,19 +8504,19 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>43</v>
@@ -8440,11 +8533,11 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
@@ -8457,24 +8550,26 @@
         <v>43</v>
       </c>
       <c r="H62" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J62" t="s" s="2">
         <v>96</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>97</v>
+        <v>198</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>121</v>
+        <v>199</v>
       </c>
       <c r="M62" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="N62" s="2"/>
+      <c r="N62" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="O62" t="s" s="2">
         <v>43</v>
       </c>
@@ -8522,7 +8617,7 @@
         <v>43</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>125</v>
+        <v>200</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8540,7 +8635,7 @@
         <v>43</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>43</v>
@@ -8551,43 +8646,41 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
-        <v>197</v>
+        <v>375</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H63" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I63" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>96</v>
+        <v>376</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>198</v>
+        <v>377</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>199</v>
+        <v>378</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N63" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>43</v>
       </c>
@@ -8635,36 +8728,36 @@
         <v>43</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>200</v>
+        <v>374</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>43</v>
+        <v>379</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>93</v>
+        <v>380</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>43</v>
+        <v>362</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>43</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8687,13 +8780,13 @@
         <v>43</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8720,13 +8813,13 @@
         <v>43</v>
       </c>
       <c r="W64" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>43</v>
+        <v>385</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>43</v>
+        <v>386</v>
       </c>
       <c r="Z64" t="s" s="2">
         <v>43</v>
@@ -8744,7 +8837,7 @@
         <v>43</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8762,18 +8855,18 @@
         <v>43</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>382</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8796,13 +8889,13 @@
         <v>43</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8853,7 +8946,7 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8871,7 +8964,7 @@
         <v>43</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>43</v>
@@ -8882,7 +8975,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8893,7 +8986,7 @@
         <v>41</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>43</v>
@@ -8905,15 +8998,17 @@
         <v>43</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>137</v>
+        <v>393</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="M66" s="2"/>
+        <v>395</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>396</v>
+      </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>43</v>
@@ -8938,37 +9033,37 @@
         <v>43</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>391</v>
+        <v>43</v>
       </c>
       <c r="Y66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE66" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="Z66" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA66" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE66" t="s" s="2">
-        <v>388</v>
-      </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>43</v>
@@ -8980,18 +9075,18 @@
         <v>43</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>394</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="67" hidden="true">
+    <row r="67">
       <c r="A67" t="s" s="2">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9005,7 +9100,7 @@
         <v>50</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H67" t="s" s="2">
         <v>43</v>
@@ -9014,15 +9109,17 @@
         <v>43</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="M67" s="2"/>
+        <v>400</v>
+      </c>
+      <c r="M67" t="s" s="2">
+        <v>401</v>
+      </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>43</v>
@@ -9047,31 +9144,31 @@
         <v>43</v>
       </c>
       <c r="W67" t="s" s="2">
-        <v>239</v>
+        <v>43</v>
       </c>
       <c r="X67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE67" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="Y67" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -9089,18 +9186,18 @@
         <v>43</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>119</v>
+        <v>402</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>400</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9111,7 +9208,7 @@
         <v>41</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>43</v>
@@ -9123,20 +9220,16 @@
         <v>43</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>137</v>
+        <v>52</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>402</v>
+        <v>116</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>405</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
         <v>43</v>
       </c>
@@ -9160,13 +9253,13 @@
         <v>43</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>239</v>
+        <v>43</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>406</v>
+        <v>43</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>407</v>
+        <v>43</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>43</v>
@@ -9184,40 +9277,40 @@
         <v>43</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>401</v>
+        <v>118</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>408</v>
+        <v>119</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>409</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
@@ -9236,15 +9329,17 @@
         <v>43</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>411</v>
+        <v>97</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="M69" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>99</v>
+      </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>43</v>
@@ -9269,13 +9364,13 @@
         <v>43</v>
       </c>
       <c r="W69" t="s" s="2">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="X69" t="s" s="2">
-        <v>413</v>
+        <v>43</v>
       </c>
       <c r="Y69" t="s" s="2">
-        <v>414</v>
+        <v>43</v>
       </c>
       <c r="Z69" t="s" s="2">
         <v>43</v>
@@ -9293,7 +9388,7 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>410</v>
+        <v>125</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -9305,28 +9400,28 @@
         <v>43</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>415</v>
+        <v>119</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>416</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>43</v>
+        <v>197</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
@@ -9339,22 +9434,26 @@
         <v>43</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I70" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>418</v>
+        <v>198</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
+        <v>199</v>
+      </c>
+      <c r="M70" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N70" t="s" s="2">
+        <v>105</v>
+      </c>
       <c r="O70" t="s" s="2">
         <v>43</v>
       </c>
@@ -9378,13 +9477,13 @@
         <v>43</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>420</v>
+        <v>43</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>421</v>
+        <v>43</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>43</v>
@@ -9402,7 +9501,7 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>417</v>
+        <v>200</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -9414,24 +9513,24 @@
         <v>43</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="AJ70" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>422</v>
+        <v>93</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>423</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9454,13 +9553,13 @@
         <v>43</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>384</v>
+        <v>108</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -9511,7 +9610,7 @@
         <v>43</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9529,18 +9628,18 @@
         <v>43</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>427</v>
+        <v>112</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>428</v>
+        <v>409</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9554,7 +9653,7 @@
         <v>50</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H72" t="s" s="2">
         <v>43</v>
@@ -9563,13 +9662,13 @@
         <v>43</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>137</v>
+        <v>411</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -9596,13 +9695,13 @@
         <v>43</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>239</v>
+        <v>43</v>
       </c>
       <c r="X72" t="s" s="2">
-        <v>432</v>
+        <v>43</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>433</v>
+        <v>43</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>43</v>
@@ -9620,7 +9719,7 @@
         <v>43</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
@@ -9638,18 +9737,18 @@
         <v>43</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>435</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9660,10 +9759,10 @@
         <v>41</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G73" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H73" t="s" s="2">
         <v>43</v>
@@ -9672,17 +9771,15 @@
         <v>43</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>439</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
         <v>43</v>
@@ -9707,13 +9804,13 @@
         <v>43</v>
       </c>
       <c r="W73" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="X73" t="s" s="2">
-        <v>43</v>
+        <v>418</v>
       </c>
       <c r="Y73" t="s" s="2">
-        <v>43</v>
+        <v>419</v>
       </c>
       <c r="Z73" t="s" s="2">
         <v>43</v>
@@ -9731,13 +9828,13 @@
         <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG73" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH73" t="s" s="2">
         <v>43</v>
@@ -9749,18 +9846,18 @@
         <v>43</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>43</v>
+        <v>421</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9783,13 +9880,13 @@
         <v>43</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>116</v>
+        <v>423</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>117</v>
+        <v>424</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9816,13 +9913,13 @@
         <v>43</v>
       </c>
       <c r="W74" t="s" s="2">
-        <v>43</v>
+        <v>239</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>43</v>
+        <v>425</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>43</v>
+        <v>426</v>
       </c>
       <c r="Z74" t="s" s="2">
         <v>43</v>
@@ -9840,7 +9937,7 @@
         <v>43</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>118</v>
+        <v>422</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9852,7 +9949,7 @@
         <v>43</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="AJ74" t="s" s="2">
         <v>43</v>
@@ -9864,16 +9961,16 @@
         <v>43</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>43</v>
+        <v>427</v>
       </c>
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
@@ -9892,18 +9989,20 @@
         <v>43</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>97</v>
+        <v>429</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>121</v>
+        <v>430</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N75" s="2"/>
+        <v>431</v>
+      </c>
+      <c r="N75" t="s" s="2">
+        <v>432</v>
+      </c>
       <c r="O75" t="s" s="2">
         <v>43</v>
       </c>
@@ -9927,13 +10026,13 @@
         <v>43</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>43</v>
+        <v>239</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>43</v>
+        <v>433</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>43</v>
+        <v>434</v>
       </c>
       <c r="Z75" t="s" s="2">
         <v>43</v>
@@ -9951,7 +10050,7 @@
         <v>43</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>125</v>
+        <v>428</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
@@ -9963,28 +10062,28 @@
         <v>43</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ75" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>119</v>
+        <v>435</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>43</v>
+        <v>436</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>197</v>
+        <v>43</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
@@ -9997,26 +10096,22 @@
         <v>43</v>
       </c>
       <c r="H76" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I76" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>198</v>
+        <v>438</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>105</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
         <v>43</v>
       </c>
@@ -10040,13 +10135,13 @@
         <v>43</v>
       </c>
       <c r="W76" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="X76" t="s" s="2">
-        <v>43</v>
+        <v>440</v>
       </c>
       <c r="Y76" t="s" s="2">
-        <v>43</v>
+        <v>441</v>
       </c>
       <c r="Z76" t="s" s="2">
         <v>43</v>
@@ -10064,7 +10159,7 @@
         <v>43</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>200</v>
+        <v>437</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -10076,22 +10171,22 @@
         <v>43</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ76" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>93</v>
+        <v>442</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>43</v>
+        <v>443</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
         <v>444</v>
       </c>
@@ -10101,13 +10196,13 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>43</v>
@@ -10116,13 +10211,13 @@
         <v>43</v>
       </c>
       <c r="J77" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="K77" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="K77" t="s" s="2">
+      <c r="L77" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>447</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -10149,13 +10244,13 @@
         <v>43</v>
       </c>
       <c r="W77" t="s" s="2">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>43</v>
+        <v>447</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>43</v>
+        <v>448</v>
       </c>
       <c r="Z77" t="s" s="2">
         <v>43</v>
@@ -10176,10 +10271,10 @@
         <v>444</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG77" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH77" t="s" s="2">
         <v>43</v>
@@ -10188,13 +10283,13 @@
         <v>62</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>448</v>
+        <v>43</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>301</v>
+        <v>449</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>449</v>
+        <v>43</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>450</v>
@@ -10225,7 +10320,7 @@
         <v>43</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>70</v>
+        <v>411</v>
       </c>
       <c r="K78" t="s" s="2">
         <v>452</v>
@@ -10233,9 +10328,7 @@
       <c r="L78" t="s" s="2">
         <v>453</v>
       </c>
-      <c r="M78" t="s" s="2">
-        <v>454</v>
-      </c>
+      <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" t="s" s="2">
         <v>43</v>
@@ -10260,13 +10353,13 @@
         <v>43</v>
       </c>
       <c r="W78" t="s" s="2">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="X78" t="s" s="2">
-        <v>455</v>
+        <v>43</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>456</v>
+        <v>43</v>
       </c>
       <c r="Z78" t="s" s="2">
         <v>43</v>
@@ -10302,18 +10395,18 @@
         <v>43</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>43</v>
+        <v>455</v>
       </c>
     </row>
-    <row r="79" hidden="true">
+    <row r="79">
       <c r="A79" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10327,7 +10420,7 @@
         <v>50</v>
       </c>
       <c r="G79" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H79" t="s" s="2">
         <v>43</v>
@@ -10339,14 +10432,12 @@
         <v>137</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>461</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
         <v>43</v>
@@ -10374,10 +10465,10 @@
         <v>239</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="Z79" t="s" s="2">
         <v>43</v>
@@ -10395,7 +10486,7 @@
         <v>43</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
@@ -10413,18 +10504,18 @@
         <v>43</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>43</v>
+        <v>461</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>43</v>
+        <v>462</v>
       </c>
     </row>
-    <row r="80" hidden="true">
+    <row r="80">
       <c r="A80" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10432,13 +10523,13 @@
       </c>
       <c r="D80" s="2"/>
       <c r="E80" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H80" t="s" s="2">
         <v>43</v>
@@ -10447,15 +10538,17 @@
         <v>43</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="K80" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="L80" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>466</v>
       </c>
-      <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
         <v>43</v>
@@ -10504,13 +10597,13 @@
         <v>43</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG80" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH80" t="s" s="2">
         <v>43</v>
@@ -10522,7 +10615,7 @@
         <v>43</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>294</v>
+        <v>467</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>43</v>
@@ -10533,7 +10626,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10556,13 +10649,13 @@
         <v>43</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>172</v>
+        <v>52</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>468</v>
+        <v>116</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>469</v>
+        <v>117</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -10613,7 +10706,7 @@
         <v>43</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>467</v>
+        <v>118</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
@@ -10625,35 +10718,35 @@
         <v>43</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>300</v>
+        <v>43</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>470</v>
+        <v>119</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>471</v>
+        <v>43</v>
       </c>
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F82" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G82" t="s" s="2">
         <v>43</v>
@@ -10665,16 +10758,16 @@
         <v>43</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>473</v>
+        <v>96</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>474</v>
+        <v>97</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>475</v>
+        <v>121</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>476</v>
+        <v>99</v>
       </c>
       <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
@@ -10724,35 +10817,808 @@
         <v>43</v>
       </c>
       <c r="AE82" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AF82" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG82" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH82" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI82" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="AJ82" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK82" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="AL82" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM82" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="83" hidden="true">
+      <c r="A83" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F83" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H83" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="I83" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J83" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="K83" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L83" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="M83" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N83" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="O83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P83" s="2"/>
+      <c r="Q83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE83" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AF83" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG83" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI83" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="AJ83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK83" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="AL83" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM83" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="B84" s="2"/>
+      <c r="C84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="F84" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G84" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="H84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J84" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="AF82" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG82" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI82" t="s" s="2">
+      <c r="K84" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="L84" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P84" s="2"/>
+      <c r="Q84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE84" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AF84" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG84" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH84" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI84" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="AJ82" t="s" s="2">
+      <c r="AJ84" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="AK84" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="AL84" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="AM84" t="s" s="2">
         <v>477</v>
       </c>
-      <c r="AK82" t="s" s="2">
+    </row>
+    <row r="85" hidden="true">
+      <c r="A85" t="s" s="2">
         <v>478</v>
       </c>
-      <c r="AL82" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AM82" t="s" s="2">
+      <c r="B85" s="2"/>
+      <c r="C85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F85" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J85" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K85" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="L85" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="M85" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="N85" s="2"/>
+      <c r="O85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P85" s="2"/>
+      <c r="Q85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W85" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="X85" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="Y85" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="Z85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE85" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="AF85" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG85" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI85" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="AJ85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK85" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="AL85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM85" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" hidden="true">
+      <c r="A86" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F86" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J86" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="K86" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="L86" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="M86" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="N86" s="2"/>
+      <c r="O86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P86" s="2"/>
+      <c r="Q86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W86" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="X86" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="Y86" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="Z86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE86" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="AF86" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG86" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI86" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="AJ86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM86" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" hidden="true">
+      <c r="A87" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F87" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J87" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="K87" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="L87" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P87" s="2"/>
+      <c r="Q87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE87" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK87" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AL87" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM87" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="F88" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G88" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="H88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J88" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="K88" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="L88" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+      <c r="O88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P88" s="2"/>
+      <c r="Q88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AK88" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="AL88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM88" t="s" s="2">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="F89" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G89" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="H89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J89" t="s" s="2">
+        <v>501</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>502</v>
+      </c>
+      <c r="L89" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="M89" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="N89" s="2"/>
+      <c r="O89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P89" s="2"/>
+      <c r="Q89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE89" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="AF89" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG89" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI89" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="AJ89" t="s" s="2">
+        <v>505</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="AL89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AM89" t="s" s="2">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM82">
+  <autoFilter ref="A1:AM89">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10762,7 +11628,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI81">
+  <conditionalFormatting sqref="A2:AI88">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>